<commit_message>
Updated Dabigatran high dose management
</commit_message>
<xml_diff>
--- a/assets/Coags.xlsx
+++ b/assets/Coags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FlutterDev\Projects\wikianesthesia_mobile\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D377909-D092-4CC1-BA3B-BA6AA3E6C46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C56D439D-2946-466F-923D-6594F76875E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="118">
   <si>
     <t>Generic</t>
   </si>
@@ -450,7 +450,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -458,8 +458,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
@@ -853,7 +852,10 @@
       <c r="F7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="5" t="s">
@@ -2309,9 +2311,6 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F7:G7"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>

</xml_diff>